<commit_message>
Excel to enum + Making sure the main scenes are selected when build
</commit_message>
<xml_diff>
--- a/Assets/Data/Excel/MasterBGM.xlsx
+++ b/Assets/Data/Excel/MasterBGM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27904070-7125-4031-AACB-A0F570B18C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{032A39F2-F48F-4F11-825E-853542B2A002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>BGM_4</t>
-  </si>
-  <si>
     <t>BGM_Boss_01</t>
   </si>
   <si>
@@ -52,6 +49,9 @@
   </si>
   <si>
     <t>BGM_Boss_03</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -406,7 +406,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -428,7 +428,7 @@
         <v>1000</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -436,7 +436,7 @@
         <v>1001</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -444,7 +444,7 @@
         <v>1002</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -452,7 +452,7 @@
         <v>1003</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>